<commit_message>
update value of R5 resistor
</commit_message>
<xml_diff>
--- a/Orp-pH Board/BOM.xlsx
+++ b/Orp-pH Board/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\pH-Board\Kicad\Orp-pH Board\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\pH_Orp_Board\Orp-pH Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F26DE5-144F-4215-B624-E14B5F657308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59109A5E-2093-4BCC-94B8-F37C8C944FCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -212,9 +212,6 @@
     <t xml:space="preserve">R5, </t>
   </si>
   <si>
-    <t>350K</t>
-  </si>
-  <si>
     <t xml:space="preserve">R6, </t>
   </si>
   <si>
@@ -327,6 +324,9 @@
   </si>
   <si>
     <t>TOTAL HT€</t>
+  </si>
+  <si>
+    <t>200K</t>
   </si>
 </sst>
 </file>
@@ -1239,8 +1239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1278,10 +1278,10 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
@@ -1422,10 +1422,10 @@
         <v>24</v>
       </c>
       <c r="H7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I7" t="s">
         <v>91</v>
-      </c>
-      <c r="I7" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
@@ -1529,7 +1529,7 @@
         <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H11">
         <v>6.06</v>
@@ -1628,7 +1628,7 @@
         <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="D15" t="s">
         <v>49</v>
@@ -1649,13 +1649,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
         <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
         <v>49</v>
@@ -1676,13 +1676,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
         <v>58</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>59</v>
-      </c>
-      <c r="C17" t="s">
-        <v>60</v>
       </c>
       <c r="D17" t="s">
         <v>49</v>
@@ -1703,13 +1703,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
         <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D18" t="s">
         <v>49</v>
@@ -1730,13 +1730,13 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
         <v>43</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
         <v>49</v>
@@ -1757,13 +1757,13 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
         <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
         <v>49</v>
@@ -1784,22 +1784,22 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
         <v>43</v>
       </c>
       <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
         <v>68</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>69</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>70</v>
-      </c>
-      <c r="F21" t="s">
-        <v>71</v>
       </c>
       <c r="G21" t="s">
         <v>9</v>
@@ -1811,22 +1811,22 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
         <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" t="s">
         <v>69</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>70</v>
-      </c>
-      <c r="F22" t="s">
-        <v>71</v>
       </c>
       <c r="G22" t="s">
         <v>9</v>
@@ -1838,22 +1838,22 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s">
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" t="s">
         <v>69</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>70</v>
-      </c>
-      <c r="F23" t="s">
-        <v>71</v>
       </c>
       <c r="G23" t="s">
         <v>9</v>
@@ -1865,25 +1865,25 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
         <v>35</v>
       </c>
       <c r="C24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" t="s">
         <v>77</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>78</v>
       </c>
-      <c r="E24" t="s">
-        <v>79</v>
-      </c>
       <c r="F24" t="s">
         <v>9</v>
       </c>
       <c r="G24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H24">
         <v>5.68</v>
@@ -1895,22 +1895,22 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
         <v>43</v>
       </c>
       <c r="C25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" t="s">
         <v>81</v>
       </c>
-      <c r="D25" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>82</v>
-      </c>
-      <c r="F25" t="s">
-        <v>83</v>
       </c>
       <c r="G25" t="s">
         <v>9</v>
@@ -1925,19 +1925,19 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B26" t="s">
         <v>43</v>
       </c>
       <c r="C26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" t="s">
         <v>85</v>
-      </c>
-      <c r="D26" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" t="s">
-        <v>86</v>
       </c>
       <c r="F26" t="s">
         <v>9</v>
@@ -1955,7 +1955,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="H28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I28">
         <f>SUM(I8:I26)</f>

</xml_diff>